<commit_message>
Added references of the datasets to the Rmd file.
</commit_message>
<xml_diff>
--- a/Data/Grounds2022.xlsx
+++ b/Data/Grounds2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeladuarte/Documents/RWork/VersionControl/AbortionLaws/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE1EF7-BAEE-5A4D-AE1B-389823F9047B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEFACE-727E-9946-BA59-A020AA4D1043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12760" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12760" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3467" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3701" uniqueCount="661">
   <si>
     <t>Region</t>
   </si>
@@ -2024,6 +2024,9 @@
   </si>
   <si>
     <t>GB</t>
+  </si>
+  <si>
+    <t>1j. On request (Yes/No/Law Varies By Jurisdiction)</t>
   </si>
 </sst>
 </file>
@@ -2078,7 +2081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2088,6 +2091,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2393,18 +2399,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O280"/>
+  <dimension ref="A1:P280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView tabSelected="1" topLeftCell="J279" workbookViewId="0">
+      <selection activeCell="N280" sqref="N280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="12" customWidth="1"/>
+    <col min="1" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2448,10 +2454,13 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="256" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="256" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -2494,11 +2503,14 @@
       <c r="N2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="240" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="240" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2541,11 +2553,14 @@
       <c r="N3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2586,9 +2601,12 @@
       <c r="N4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -2625,11 +2643,12 @@
         <v>18</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="4"/>
+      <c r="P5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -2672,11 +2691,14 @@
       <c r="N6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2719,11 +2741,14 @@
       <c r="N7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="144" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="144" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2766,11 +2791,14 @@
       <c r="N8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -2813,9 +2841,12 @@
       <c r="N9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+      <c r="O9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -2856,11 +2887,14 @@
       <c r="N10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -2903,11 +2937,14 @@
       <c r="N11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -2950,11 +2987,14 @@
       <c r="N12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2997,9 +3037,12 @@
       <c r="N13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -3042,11 +3085,14 @@
       <c r="N14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -3089,11 +3135,14 @@
       <c r="N15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="192" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="192" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -3136,11 +3185,14 @@
       <c r="N16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -3183,9 +3235,12 @@
       <c r="N17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -3210,9 +3265,10 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+      <c r="O18" s="4"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -3255,11 +3311,14 @@
       <c r="N19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -3302,11 +3361,14 @@
       <c r="N20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="O20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="380" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="380" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -3349,11 +3411,14 @@
       <c r="N21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="O21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P21" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -3396,11 +3461,14 @@
       <c r="N22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="O22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -3429,11 +3497,12 @@
         <v>18</v>
       </c>
       <c r="N23" s="3"/>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="4"/>
+      <c r="P23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
@@ -3476,11 +3545,14 @@
       <c r="N24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
@@ -3523,11 +3595,14 @@
       <c r="N25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="O25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
@@ -3552,11 +3627,12 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3" t="s">
+      <c r="O26" s="4"/>
+      <c r="P26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="395" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="395" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
@@ -3589,11 +3665,12 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="3" t="s">
+      <c r="O27" s="4"/>
+      <c r="P27" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
@@ -3636,11 +3713,14 @@
       <c r="N28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="O28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="224" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="224" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>14</v>
       </c>
@@ -3675,11 +3755,12 @@
         <v>18</v>
       </c>
       <c r="N29" s="3"/>
-      <c r="O29" s="3" t="s">
+      <c r="O29" s="4"/>
+      <c r="P29" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
@@ -3722,11 +3803,14 @@
       <c r="N30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O30" s="3" t="s">
+      <c r="O30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
@@ -3769,11 +3853,14 @@
       <c r="N31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P31" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -3816,11 +3903,14 @@
       <c r="N32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O32" s="3" t="s">
+      <c r="O32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P32" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -3863,11 +3953,14 @@
       <c r="N33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O33" s="3" t="s">
+      <c r="O33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P33" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="160" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="160" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
@@ -3910,11 +4003,14 @@
       <c r="N34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O34" s="3" t="s">
+      <c r="O34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P34" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>14</v>
       </c>
@@ -3957,9 +4053,12 @@
       <c r="N35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -4002,11 +4101,14 @@
       <c r="N36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="O36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P36" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
@@ -4049,11 +4151,14 @@
       <c r="N37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="O37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P37" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
@@ -4096,11 +4201,14 @@
       <c r="N38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O38" s="3" t="s">
+      <c r="O38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P38" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
@@ -4143,11 +4251,14 @@
       <c r="N39" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O39" s="3" t="s">
+      <c r="O39" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P39" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
@@ -4188,11 +4299,14 @@
       <c r="N40" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O40" s="3" t="s">
+      <c r="O40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P40" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
@@ -4219,11 +4333,12 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="3" t="s">
+      <c r="O41" s="4"/>
+      <c r="P41" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
@@ -4266,9 +4381,12 @@
       <c r="N42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O42" s="3"/>
-    </row>
-    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>14</v>
       </c>
@@ -4311,11 +4429,14 @@
       <c r="N43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O43" s="3" t="s">
+      <c r="O43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P43" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -4356,9 +4477,12 @@
       <c r="N44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O44" s="3"/>
-    </row>
-    <row r="45" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -4397,11 +4521,12 @@
         <v>18</v>
       </c>
       <c r="N45" s="3"/>
-      <c r="O45" s="3" t="s">
+      <c r="O45" s="4"/>
+      <c r="P45" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>14</v>
       </c>
@@ -4426,9 +4551,10 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-    </row>
-    <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O46" s="4"/>
+      <c r="P46" s="3"/>
+    </row>
+    <row r="47" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
@@ -4471,11 +4597,14 @@
       <c r="N47" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O47" s="3" t="s">
+      <c r="O47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P47" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
@@ -4516,11 +4645,14 @@
       <c r="N48" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O48" s="3" t="s">
+      <c r="O48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P48" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
@@ -4563,11 +4695,14 @@
       <c r="N49" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O49" s="3" t="s">
+      <c r="O49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P49" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>14</v>
       </c>
@@ -4610,9 +4745,12 @@
       <c r="N50" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O50" s="3"/>
-    </row>
-    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P50" s="3"/>
+    </row>
+    <row r="51" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>14</v>
       </c>
@@ -4655,9 +4793,12 @@
       <c r="N51" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O51" s="3"/>
-    </row>
-    <row r="52" spans="1:15" ht="160" x14ac:dyDescent="0.2">
+      <c r="O51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P51" s="3"/>
+    </row>
+    <row r="52" spans="1:16" ht="160" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
@@ -4698,11 +4839,14 @@
       <c r="N52" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O52" s="3" t="s">
+      <c r="O52" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P52" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -4729,11 +4873,12 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
-      <c r="O53" s="3" t="s">
+      <c r="O53" s="4"/>
+      <c r="P53" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
@@ -4760,9 +4905,10 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-    </row>
-    <row r="55" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O54" s="4"/>
+      <c r="P54" s="3"/>
+    </row>
+    <row r="55" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
@@ -4805,11 +4951,14 @@
       <c r="N55" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O55" s="3" t="s">
+      <c r="O55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P55" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>118</v>
       </c>
@@ -4852,9 +5001,12 @@
       <c r="N56" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O56" s="3"/>
-    </row>
-    <row r="57" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P56" s="3"/>
+    </row>
+    <row r="57" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>118</v>
       </c>
@@ -4881,11 +5033,14 @@
       <c r="N57" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O57" s="3" t="s">
+      <c r="O57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P57" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>118</v>
       </c>
@@ -4910,11 +5065,14 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
-      <c r="O58" s="3" t="s">
+      <c r="O58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P58" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>118</v>
       </c>
@@ -4957,9 +5115,12 @@
       <c r="N59" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O59" s="3"/>
-    </row>
-    <row r="60" spans="1:15" ht="160" x14ac:dyDescent="0.2">
+      <c r="O59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" ht="160" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>118</v>
       </c>
@@ -5002,11 +5163,14 @@
       <c r="N60" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O60" s="3" t="s">
+      <c r="O60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P60" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>118</v>
       </c>
@@ -5049,9 +5213,12 @@
       <c r="N61" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O61" s="3"/>
-    </row>
-    <row r="62" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P61" s="3"/>
+    </row>
+    <row r="62" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>118</v>
       </c>
@@ -5094,11 +5261,14 @@
       <c r="N62" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O62" s="3" t="s">
+      <c r="O62" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P62" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>118</v>
       </c>
@@ -5129,11 +5299,14 @@
         <v>18</v>
       </c>
       <c r="N63" s="3"/>
-      <c r="O63" s="3" t="s">
+      <c r="O63" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P63" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>118</v>
       </c>
@@ -5166,11 +5339,14 @@
         <v>18</v>
       </c>
       <c r="N64" s="3"/>
-      <c r="O64" s="3" t="s">
+      <c r="O64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P64" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="96" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>118</v>
       </c>
@@ -5207,11 +5383,12 @@
         <v>18</v>
       </c>
       <c r="N65" s="3"/>
-      <c r="O65" s="3" t="s">
+      <c r="O65" s="4"/>
+      <c r="P65" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>118</v>
       </c>
@@ -5248,11 +5425,14 @@
         <v>18</v>
       </c>
       <c r="N66" s="3"/>
-      <c r="O66" s="3" t="s">
+      <c r="O66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P66" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>118</v>
       </c>
@@ -5277,9 +5457,10 @@
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-    </row>
-    <row r="68" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O67" s="4"/>
+      <c r="P67" s="3"/>
+    </row>
+    <row r="68" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>118</v>
       </c>
@@ -5312,11 +5493,14 @@
         <v>18</v>
       </c>
       <c r="N68" s="3"/>
-      <c r="O68" s="3" t="s">
+      <c r="O68" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P68" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>118</v>
       </c>
@@ -5359,11 +5543,14 @@
       <c r="N69" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O69" s="3" t="s">
+      <c r="O69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P69" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>118</v>
       </c>
@@ -5406,9 +5593,12 @@
       <c r="N70" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O70" s="3"/>
-    </row>
-    <row r="71" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O70" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P70" s="3"/>
+    </row>
+    <row r="71" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>118</v>
       </c>
@@ -5451,11 +5641,14 @@
       <c r="N71" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O71" s="3" t="s">
+      <c r="O71" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P71" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>118</v>
       </c>
@@ -5498,11 +5691,14 @@
       <c r="N72" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O72" s="3" t="s">
+      <c r="O72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P72" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="208" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="208" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>118</v>
       </c>
@@ -5545,11 +5741,14 @@
       <c r="N73" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O73" s="3" t="s">
+      <c r="O73" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P73" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>118</v>
       </c>
@@ -5592,11 +5791,14 @@
       <c r="N74" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O74" s="3" t="s">
+      <c r="O74" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P74" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>118</v>
       </c>
@@ -5639,11 +5841,14 @@
       <c r="N75" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O75" s="3" t="s">
+      <c r="O75" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P75" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>118</v>
       </c>
@@ -5676,11 +5881,14 @@
       <c r="N76" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O76" s="3" t="s">
+      <c r="O76" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P76" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>118</v>
       </c>
@@ -5723,11 +5931,14 @@
       <c r="N77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O77" s="3" t="s">
+      <c r="O77" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P77" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>118</v>
       </c>
@@ -5756,11 +5967,14 @@
         <v>18</v>
       </c>
       <c r="N78" s="3"/>
-      <c r="O78" s="3" t="s">
+      <c r="O78" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P78" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="288" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="288" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>118</v>
       </c>
@@ -5787,11 +6001,12 @@
       </c>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
-      <c r="O79" s="3" t="s">
+      <c r="O79" s="4"/>
+      <c r="P79" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>118</v>
       </c>
@@ -5818,9 +6033,10 @@
       <c r="L80" s="3"/>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-    </row>
-    <row r="81" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O80" s="4"/>
+      <c r="P80" s="3"/>
+    </row>
+    <row r="81" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>118</v>
       </c>
@@ -5863,11 +6079,14 @@
       <c r="N81" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O81" s="3" t="s">
+      <c r="O81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P81" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>118</v>
       </c>
@@ -5910,11 +6129,14 @@
       <c r="N82" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O82" s="3" t="s">
+      <c r="O82" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P82" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>118</v>
       </c>
@@ -5953,11 +6175,14 @@
         <v>18</v>
       </c>
       <c r="N83" s="3"/>
-      <c r="O83" s="3" t="s">
+      <c r="O83" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P83" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>118</v>
       </c>
@@ -6000,9 +6225,12 @@
       <c r="N84" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O84" s="3"/>
-    </row>
-    <row r="85" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O84" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P84" s="3"/>
+    </row>
+    <row r="85" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>118</v>
       </c>
@@ -6045,9 +6273,12 @@
       <c r="N85" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O85" s="3"/>
-    </row>
-    <row r="86" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="O85" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P85" s="3"/>
+    </row>
+    <row r="86" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>118</v>
       </c>
@@ -6090,11 +6321,14 @@
       <c r="N86" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O86" s="3" t="s">
+      <c r="O86" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P86" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="96" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>118</v>
       </c>
@@ -6137,11 +6371,14 @@
       <c r="N87" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O87" s="3" t="s">
+      <c r="O87" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P87" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>118</v>
       </c>
@@ -6184,11 +6421,14 @@
       <c r="N88" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O88" s="3" t="s">
+      <c r="O88" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P88" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>118</v>
       </c>
@@ -6231,11 +6471,14 @@
       <c r="N89" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O89" s="3" t="s">
+      <c r="O89" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P89" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>118</v>
       </c>
@@ -6278,11 +6521,14 @@
       <c r="N90" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O90" s="3" t="s">
+      <c r="O90" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P90" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="395" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="395" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>118</v>
       </c>
@@ -6325,11 +6571,14 @@
       <c r="N91" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O91" s="3" t="s">
+      <c r="O91" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P91" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>118</v>
       </c>
@@ -6372,11 +6621,14 @@
       <c r="N92" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O92" s="3" t="s">
+      <c r="O92" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P92" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>118</v>
       </c>
@@ -6419,9 +6671,12 @@
       <c r="N93" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O93" s="3"/>
-    </row>
-    <row r="94" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O93" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P93" s="3"/>
+    </row>
+    <row r="94" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>118</v>
       </c>
@@ -6464,11 +6719,14 @@
       <c r="N94" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O94" s="3" t="s">
+      <c r="O94" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P94" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>118</v>
       </c>
@@ -6497,11 +6755,12 @@
       <c r="N95" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O95" s="3" t="s">
+      <c r="O95" s="4"/>
+      <c r="P95" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>118</v>
       </c>
@@ -6544,9 +6803,12 @@
       <c r="N96" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O96" s="3"/>
-    </row>
-    <row r="97" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+      <c r="O96" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P96" s="3"/>
+    </row>
+    <row r="97" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>118</v>
       </c>
@@ -6589,11 +6851,14 @@
       <c r="N97" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O97" s="3" t="s">
+      <c r="O97" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P97" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>118</v>
       </c>
@@ -6636,11 +6901,14 @@
       <c r="N98" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O98" s="3" t="s">
+      <c r="O98" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P98" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>118</v>
       </c>
@@ -6669,11 +6937,14 @@
       <c r="N99" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O99" s="3" t="s">
+      <c r="O99" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P99" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>118</v>
       </c>
@@ -6716,11 +6987,14 @@
       <c r="N100" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O100" s="3" t="s">
+      <c r="O100" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P100" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>118</v>
       </c>
@@ -6755,11 +7029,14 @@
       <c r="N101" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O101" s="3" t="s">
+      <c r="O101" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P101" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>118</v>
       </c>
@@ -6784,11 +7061,14 @@
       <c r="L102" s="3"/>
       <c r="M102" s="3"/>
       <c r="N102" s="3"/>
-      <c r="O102" s="3" t="s">
+      <c r="O102" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P102" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>118</v>
       </c>
@@ -6831,11 +7111,14 @@
       <c r="N103" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O103" s="3" t="s">
+      <c r="O103" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P103" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>196</v>
       </c>
@@ -6878,11 +7161,14 @@
       <c r="N104" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O104" s="3" t="s">
+      <c r="O104" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P104" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>196</v>
       </c>
@@ -6925,11 +7211,14 @@
       <c r="N105" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O105" s="3" t="s">
+      <c r="O105" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P105" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>196</v>
       </c>
@@ -6972,11 +7261,14 @@
       <c r="N106" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O106" s="3" t="s">
+      <c r="O106" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P106" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>196</v>
       </c>
@@ -7007,11 +7299,14 @@
       <c r="N107" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O107" s="3" t="s">
+      <c r="O107" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P107" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="208" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" ht="208" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>196</v>
       </c>
@@ -7054,11 +7349,14 @@
       <c r="N108" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O108" s="3" t="s">
+      <c r="O108" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P108" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>196</v>
       </c>
@@ -7101,9 +7399,12 @@
       <c r="N109" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O109" s="3"/>
-    </row>
-    <row r="110" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O109" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P109" s="3"/>
+    </row>
+    <row r="110" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>196</v>
       </c>
@@ -7128,9 +7429,10 @@
       <c r="L110" s="3"/>
       <c r="M110" s="3"/>
       <c r="N110" s="3"/>
-      <c r="O110" s="3"/>
-    </row>
-    <row r="111" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+      <c r="O110" s="4"/>
+      <c r="P110" s="3"/>
+    </row>
+    <row r="111" spans="1:16" ht="96" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>196</v>
       </c>
@@ -7173,11 +7475,14 @@
       <c r="N111" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O111" s="3" t="s">
+      <c r="O111" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P111" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>196</v>
       </c>
@@ -7208,11 +7513,14 @@
       <c r="L112" s="3"/>
       <c r="M112" s="3"/>
       <c r="N112" s="3"/>
-      <c r="O112" s="3" t="s">
+      <c r="O112" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P112" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>196</v>
       </c>
@@ -7247,9 +7555,12 @@
         <v>18</v>
       </c>
       <c r="N113" s="3"/>
-      <c r="O113" s="3"/>
-    </row>
-    <row r="114" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+      <c r="O113" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P113" s="3"/>
+    </row>
+    <row r="114" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>196</v>
       </c>
@@ -7282,11 +7593,14 @@
         <v>18</v>
       </c>
       <c r="N114" s="3"/>
-      <c r="O114" s="3" t="s">
+      <c r="O114" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P114" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>196</v>
       </c>
@@ -7327,11 +7641,14 @@
       <c r="N115" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O115" s="3" t="s">
+      <c r="O115" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P115" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>196</v>
       </c>
@@ -7364,11 +7681,14 @@
         <v>18</v>
       </c>
       <c r="N116" s="3"/>
-      <c r="O116" s="3" t="s">
+      <c r="O116" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P116" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="256" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" ht="256" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>196</v>
       </c>
@@ -7407,11 +7727,12 @@
       <c r="N117" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O117" s="3" t="s">
+      <c r="O117" s="4"/>
+      <c r="P117" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="240" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" ht="240" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>196</v>
       </c>
@@ -7440,11 +7761,14 @@
         <v>18</v>
       </c>
       <c r="N118" s="3"/>
-      <c r="O118" s="3" t="s">
+      <c r="O118" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P118" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="380" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" ht="380" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>196</v>
       </c>
@@ -7485,11 +7809,14 @@
         <v>19</v>
       </c>
       <c r="N119" s="3"/>
-      <c r="O119" s="3" t="s">
+      <c r="O119" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P119" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="192" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" ht="192" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>196</v>
       </c>
@@ -7532,11 +7859,14 @@
       <c r="N120" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O120" s="3" t="s">
+      <c r="O120" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P120" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>196</v>
       </c>
@@ -7579,11 +7909,14 @@
       <c r="N121" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O121" s="3" t="s">
+      <c r="O121" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P121" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>196</v>
       </c>
@@ -7626,11 +7959,14 @@
       <c r="N122" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O122" s="3" t="s">
+      <c r="O122" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P122" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>196</v>
       </c>
@@ -7659,11 +7995,14 @@
         <v>18</v>
       </c>
       <c r="N123" s="3"/>
-      <c r="O123" s="3" t="s">
+      <c r="O123" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P123" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="160" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" ht="160" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>196</v>
       </c>
@@ -7706,11 +8045,14 @@
       <c r="N124" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O124" s="3" t="s">
+      <c r="O124" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P124" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>196</v>
       </c>
@@ -7753,11 +8095,14 @@
       <c r="N125" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O125" s="3" t="s">
+      <c r="O125" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P125" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>196</v>
       </c>
@@ -7784,11 +8129,14 @@
       </c>
       <c r="M126" s="3"/>
       <c r="N126" s="3"/>
-      <c r="O126" s="3" t="s">
+      <c r="O126" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P126" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="256" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" ht="256" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>196</v>
       </c>
@@ -7831,11 +8179,14 @@
       <c r="N127" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O127" s="3" t="s">
+      <c r="O127" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P127" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="320" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" ht="320" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>196</v>
       </c>
@@ -7866,11 +8217,14 @@
       <c r="L128" s="3"/>
       <c r="M128" s="3"/>
       <c r="N128" s="3"/>
-      <c r="O128" s="3" t="s">
+      <c r="O128" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P128" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>196</v>
       </c>
@@ -7913,11 +8267,14 @@
       <c r="N129" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O129" s="3" t="s">
+      <c r="O129" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P129" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>196</v>
       </c>
@@ -7960,11 +8317,14 @@
       <c r="N130" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O130" s="3" t="s">
+      <c r="O130" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P130" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>196</v>
       </c>
@@ -8007,11 +8367,14 @@
       <c r="N131" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O131" s="3" t="s">
+      <c r="O131" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P131" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="144" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" ht="144" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>196</v>
       </c>
@@ -8046,11 +8409,14 @@
         <v>18</v>
       </c>
       <c r="N132" s="3"/>
-      <c r="O132" s="3" t="s">
+      <c r="O132" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P132" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>196</v>
       </c>
@@ -8093,11 +8459,14 @@
       <c r="N133" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O133" s="3" t="s">
+      <c r="O133" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P133" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>196</v>
       </c>
@@ -8140,9 +8509,12 @@
       <c r="N134" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O134" s="3"/>
-    </row>
-    <row r="135" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O134" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P134" s="3"/>
+    </row>
+    <row r="135" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>196</v>
       </c>
@@ -8183,11 +8555,14 @@
       <c r="N135" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O135" s="3" t="s">
+      <c r="O135" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P135" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>196</v>
       </c>
@@ -8230,9 +8605,12 @@
       <c r="N136" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O136" s="3"/>
-    </row>
-    <row r="137" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+      <c r="O136" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P136" s="3"/>
+    </row>
+    <row r="137" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>196</v>
       </c>
@@ -8275,11 +8653,14 @@
       <c r="N137" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O137" s="3" t="s">
+      <c r="O137" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P137" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>196</v>
       </c>
@@ -8316,11 +8697,14 @@
         <v>18</v>
       </c>
       <c r="N138" s="3"/>
-      <c r="O138" s="3" t="s">
+      <c r="O138" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P138" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>196</v>
       </c>
@@ -8363,11 +8747,14 @@
       <c r="N139" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O139" s="3" t="s">
+      <c r="O139" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P139" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>196</v>
       </c>
@@ -8398,11 +8785,14 @@
       <c r="N140" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O140" s="3" t="s">
+      <c r="O140" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P140" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>196</v>
       </c>
@@ -8445,11 +8835,14 @@
       <c r="N141" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O141" s="3" t="s">
+      <c r="O141" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P141" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>196</v>
       </c>
@@ -8492,11 +8885,14 @@
       <c r="N142" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O142" s="3" t="s">
+      <c r="O142" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P142" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>196</v>
       </c>
@@ -8539,11 +8935,14 @@
       <c r="N143" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O143" s="3" t="s">
+      <c r="O143" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P143" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>196</v>
       </c>
@@ -8572,11 +8971,14 @@
       <c r="L144" s="3"/>
       <c r="M144" s="3"/>
       <c r="N144" s="3"/>
-      <c r="O144" s="3" t="s">
+      <c r="O144" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P144" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>196</v>
       </c>
@@ -8619,11 +9021,14 @@
       <c r="N145" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O145" s="3" t="s">
+      <c r="O145" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P145" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>196</v>
       </c>
@@ -8652,9 +9057,12 @@
       <c r="L146" s="3"/>
       <c r="M146" s="3"/>
       <c r="N146" s="3"/>
-      <c r="O146" s="3"/>
-    </row>
-    <row r="147" spans="1:15" ht="395" x14ac:dyDescent="0.2">
+      <c r="O146" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P146" s="3"/>
+    </row>
+    <row r="147" spans="1:16" ht="395" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>196</v>
       </c>
@@ -8697,11 +9105,14 @@
       <c r="N147" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O147" s="3" t="s">
+      <c r="O147" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P147" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>196</v>
       </c>
@@ -8744,11 +9155,14 @@
       <c r="N148" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O148" s="3" t="s">
+      <c r="O148" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P148" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>196</v>
       </c>
@@ -8791,11 +9205,14 @@
       <c r="N149" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O149" s="3" t="s">
+      <c r="O149" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P149" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>196</v>
       </c>
@@ -8838,11 +9255,14 @@
       <c r="N150" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O150" s="3" t="s">
+      <c r="O150" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P150" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>196</v>
       </c>
@@ -8885,11 +9305,14 @@
       <c r="N151" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O151" s="3" t="s">
+      <c r="O151" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P151" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>196</v>
       </c>
@@ -8932,11 +9355,14 @@
       <c r="N152" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O152" s="3" t="s">
+      <c r="O152" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P152" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>196</v>
       </c>
@@ -8979,11 +9405,14 @@
       <c r="N153" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O153" s="3" t="s">
+      <c r="O153" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P153" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>196</v>
       </c>
@@ -9026,11 +9455,14 @@
       <c r="N154" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O154" s="3" t="s">
+      <c r="O154" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P154" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>196</v>
       </c>
@@ -9073,11 +9505,14 @@
       <c r="N155" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O155" s="3" t="s">
+      <c r="O155" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P155" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>196</v>
       </c>
@@ -9120,11 +9555,14 @@
       <c r="N156" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O156" s="3" t="s">
+      <c r="O156" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P156" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>196</v>
       </c>
@@ -9167,11 +9605,14 @@
       <c r="N157" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O157" s="3" t="s">
+      <c r="O157" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P157" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>196</v>
       </c>
@@ -9214,11 +9655,14 @@
       <c r="N158" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O158" s="3" t="s">
+      <c r="O158" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P158" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>196</v>
       </c>
@@ -9261,11 +9705,14 @@
       <c r="N159" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O159" s="3" t="s">
+      <c r="O159" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P159" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>196</v>
       </c>
@@ -9308,11 +9755,14 @@
       <c r="N160" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O160" s="3" t="s">
+      <c r="O160" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P160" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>196</v>
       </c>
@@ -9355,11 +9805,14 @@
       <c r="N161" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O161" s="3" t="s">
+      <c r="O161" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P161" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>196</v>
       </c>
@@ -9402,11 +9855,14 @@
       <c r="N162" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O162" s="3" t="s">
+      <c r="O162" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P162" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>196</v>
       </c>
@@ -9449,11 +9905,14 @@
       <c r="N163" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O163" s="3" t="s">
+      <c r="O163" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P163" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>196</v>
       </c>
@@ -9496,11 +9955,14 @@
       <c r="N164" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O164" s="3" t="s">
+      <c r="O164" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P164" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>196</v>
       </c>
@@ -9543,11 +10005,14 @@
       <c r="N165" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O165" s="3" t="s">
+      <c r="O165" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P165" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>196</v>
       </c>
@@ -9590,11 +10055,14 @@
       <c r="N166" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O166" s="3" t="s">
+      <c r="O166" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P166" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>196</v>
       </c>
@@ -9637,11 +10105,14 @@
       <c r="N167" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O167" s="3" t="s">
+      <c r="O167" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P167" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>196</v>
       </c>
@@ -9684,11 +10155,14 @@
       <c r="N168" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O168" s="3" t="s">
+      <c r="O168" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P168" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>196</v>
       </c>
@@ -9731,11 +10205,14 @@
       <c r="N169" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O169" s="3" t="s">
+      <c r="O169" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P169" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>196</v>
       </c>
@@ -9778,11 +10255,14 @@
       <c r="N170" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O170" s="3" t="s">
+      <c r="O170" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P170" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>196</v>
       </c>
@@ -9825,11 +10305,14 @@
       <c r="N171" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O171" s="3" t="s">
+      <c r="O171" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P171" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>196</v>
       </c>
@@ -9872,11 +10355,14 @@
       <c r="N172" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O172" s="3" t="s">
+      <c r="O172" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P172" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>196</v>
       </c>
@@ -9911,11 +10397,14 @@
         <v>18</v>
       </c>
       <c r="N173" s="3"/>
-      <c r="O173" s="3" t="s">
+      <c r="O173" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P173" s="3" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="304" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" ht="304" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>196</v>
       </c>
@@ -9948,11 +10437,12 @@
         <v>18</v>
       </c>
       <c r="N174" s="3"/>
-      <c r="O174" s="3" t="s">
+      <c r="O174" s="4"/>
+      <c r="P174" s="3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="304" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" ht="304" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>196</v>
       </c>
@@ -9985,11 +10475,12 @@
         <v>18</v>
       </c>
       <c r="N175" s="3"/>
-      <c r="O175" s="3" t="s">
+      <c r="O175" s="4"/>
+      <c r="P175" s="3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>196</v>
       </c>
@@ -10032,11 +10523,14 @@
       <c r="N176" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O176" s="3" t="s">
+      <c r="O176" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P176" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>196</v>
       </c>
@@ -10069,11 +10563,12 @@
         <v>18</v>
       </c>
       <c r="N177" s="3"/>
-      <c r="O177" s="3" t="s">
+      <c r="O177" s="4"/>
+      <c r="P177" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>196</v>
       </c>
@@ -10106,9 +10601,12 @@
         <v>18</v>
       </c>
       <c r="N178" s="3"/>
-      <c r="O178" s="3"/>
-    </row>
-    <row r="179" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O178" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P178" s="3"/>
+    </row>
+    <row r="179" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>318</v>
       </c>
@@ -10133,11 +10631,12 @@
       <c r="L179" s="3"/>
       <c r="M179" s="3"/>
       <c r="N179" s="3"/>
-      <c r="O179" s="3" t="s">
+      <c r="O179" s="4"/>
+      <c r="P179" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>318</v>
       </c>
@@ -10180,9 +10679,12 @@
       <c r="N180" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O180" s="3"/>
-    </row>
-    <row r="181" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O180" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P180" s="3"/>
+    </row>
+    <row r="181" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>318</v>
       </c>
@@ -10207,9 +10709,10 @@
       <c r="L181" s="3"/>
       <c r="M181" s="3"/>
       <c r="N181" s="3"/>
-      <c r="O181" s="3"/>
-    </row>
-    <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O181" s="4"/>
+      <c r="P181" s="3"/>
+    </row>
+    <row r="182" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>318</v>
       </c>
@@ -10242,9 +10745,10 @@
         <v>18</v>
       </c>
       <c r="N182" s="3"/>
-      <c r="O182" s="3"/>
-    </row>
-    <row r="183" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O182" s="4"/>
+      <c r="P182" s="3"/>
+    </row>
+    <row r="183" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>318</v>
       </c>
@@ -10277,11 +10781,12 @@
         <v>18</v>
       </c>
       <c r="N183" s="3"/>
-      <c r="O183" s="3" t="s">
+      <c r="O183" s="4"/>
+      <c r="P183" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>318</v>
       </c>
@@ -10320,9 +10825,10 @@
         <v>19</v>
       </c>
       <c r="N184" s="3"/>
-      <c r="O184" s="3"/>
-    </row>
-    <row r="185" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+      <c r="O184" s="4"/>
+      <c r="P184" s="3"/>
+    </row>
+    <row r="185" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>318</v>
       </c>
@@ -10365,11 +10871,14 @@
       <c r="N185" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O185" s="3" t="s">
+      <c r="O185" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P185" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="272" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" ht="272" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>318</v>
       </c>
@@ -10412,11 +10921,14 @@
       <c r="N186" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O186" s="3" t="s">
+      <c r="O186" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P186" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="288" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" ht="288" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>318</v>
       </c>
@@ -10459,11 +10971,14 @@
       <c r="N187" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O187" s="3" t="s">
+      <c r="O187" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P187" s="3" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>318</v>
       </c>
@@ -10506,11 +11021,14 @@
       <c r="N188" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O188" s="3" t="s">
+      <c r="O188" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P188" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="176" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16" ht="176" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>318</v>
       </c>
@@ -10545,11 +11063,14 @@
       <c r="N189" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O189" s="3" t="s">
+      <c r="O189" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P189" s="3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>318</v>
       </c>
@@ -10574,11 +11095,12 @@
       <c r="L190" s="3"/>
       <c r="M190" s="3"/>
       <c r="N190" s="3"/>
-      <c r="O190" s="3" t="s">
+      <c r="O190" s="4"/>
+      <c r="P190" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>318</v>
       </c>
@@ -10621,11 +11143,14 @@
       <c r="N191" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O191" s="3" t="s">
+      <c r="O191" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P191" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>318</v>
       </c>
@@ -10668,11 +11193,14 @@
       <c r="N192" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O192" s="3" t="s">
+      <c r="O192" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P192" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>318</v>
       </c>
@@ -10715,11 +11243,14 @@
       <c r="N193" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O193" s="3" t="s">
+      <c r="O193" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P193" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="194" spans="1:15" ht="380" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" ht="380" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>318</v>
       </c>
@@ -10744,11 +11275,12 @@
       <c r="L194" s="3"/>
       <c r="M194" s="3"/>
       <c r="N194" s="3"/>
-      <c r="O194" s="3" t="s">
+      <c r="O194" s="4"/>
+      <c r="P194" s="3" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>318</v>
       </c>
@@ -10791,11 +11323,14 @@
       <c r="N195" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O195" s="3" t="s">
+      <c r="O195" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P195" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="320" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" ht="320" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>318</v>
       </c>
@@ -10834,11 +11369,14 @@
         <v>18</v>
       </c>
       <c r="N196" s="3"/>
-      <c r="O196" s="3" t="s">
+      <c r="O196" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P196" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>318</v>
       </c>
@@ -10881,11 +11419,14 @@
       <c r="N197" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O197" s="3" t="s">
+      <c r="O197" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P197" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>318</v>
       </c>
@@ -10918,11 +11459,14 @@
       <c r="N198" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O198" s="3" t="s">
+      <c r="O198" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P198" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>318</v>
       </c>
@@ -10947,11 +11491,12 @@
       <c r="L199" s="3"/>
       <c r="M199" s="3"/>
       <c r="N199" s="3"/>
-      <c r="O199" s="3" t="s">
+      <c r="O199" s="4"/>
+      <c r="P199" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>318</v>
       </c>
@@ -10994,9 +11539,12 @@
       <c r="N200" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O200" s="3"/>
-    </row>
-    <row r="201" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O200" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P200" s="3"/>
+    </row>
+    <row r="201" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>318</v>
       </c>
@@ -11039,9 +11587,12 @@
       <c r="N201" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O201" s="3"/>
-    </row>
-    <row r="202" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+      <c r="O201" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P201" s="3"/>
+    </row>
+    <row r="202" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>318</v>
       </c>
@@ -11084,11 +11635,14 @@
       <c r="N202" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O202" s="3" t="s">
+      <c r="O202" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P202" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>318</v>
       </c>
@@ -11131,11 +11685,14 @@
       <c r="N203" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O203" s="3" t="s">
+      <c r="O203" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P203" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="204" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>318</v>
       </c>
@@ -11178,9 +11735,12 @@
       <c r="N204" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O204" s="3"/>
-    </row>
-    <row r="205" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O204" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P204" s="3"/>
+    </row>
+    <row r="205" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>318</v>
       </c>
@@ -11223,9 +11783,12 @@
       <c r="N205" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O205" s="3"/>
-    </row>
-    <row r="206" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+      <c r="O205" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P205" s="3"/>
+    </row>
+    <row r="206" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>318</v>
       </c>
@@ -11268,11 +11831,14 @@
       <c r="N206" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O206" s="3" t="s">
+      <c r="O206" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P206" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="272" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" ht="272" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>318</v>
       </c>
@@ -11313,11 +11879,14 @@
       <c r="N207" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O207" s="3" t="s">
+      <c r="O207" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P207" s="3" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>318</v>
       </c>
@@ -11360,11 +11929,14 @@
       <c r="N208" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O208" s="3" t="s">
+      <c r="O208" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P208" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>318</v>
       </c>
@@ -11407,9 +11979,12 @@
       <c r="N209" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O209" s="3"/>
-    </row>
-    <row r="210" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O209" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P209" s="3"/>
+    </row>
+    <row r="210" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>318</v>
       </c>
@@ -11452,9 +12027,12 @@
       <c r="N210" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O210" s="3"/>
-    </row>
-    <row r="211" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O210" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P210" s="3"/>
+    </row>
+    <row r="211" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>318</v>
       </c>
@@ -11497,9 +12075,12 @@
       <c r="N211" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O211" s="3"/>
-    </row>
-    <row r="212" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O211" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P211" s="3"/>
+    </row>
+    <row r="212" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>318</v>
       </c>
@@ -11542,11 +12123,14 @@
       <c r="N212" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O212" s="3" t="s">
+      <c r="O212" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P212" s="3" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="208" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" ht="208" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>318</v>
       </c>
@@ -11589,11 +12173,14 @@
       <c r="N213" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O213" s="3" t="s">
+      <c r="O213" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P213" s="3" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>318</v>
       </c>
@@ -11636,9 +12223,12 @@
       <c r="N214" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O214" s="3"/>
-    </row>
-    <row r="215" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O214" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P214" s="3"/>
+    </row>
+    <row r="215" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>318</v>
       </c>
@@ -11681,11 +12271,14 @@
       <c r="N215" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O215" s="3" t="s">
+      <c r="O215" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P215" s="3" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="144" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" ht="144" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>318</v>
       </c>
@@ -11728,11 +12321,14 @@
       <c r="N216" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O216" s="3" t="s">
+      <c r="O216" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P216" s="3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>318</v>
       </c>
@@ -11775,11 +12371,14 @@
       <c r="N217" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O217" s="3" t="s">
+      <c r="O217" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P217" s="3" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>318</v>
       </c>
@@ -11822,9 +12421,12 @@
       <c r="N218" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O218" s="3"/>
-    </row>
-    <row r="219" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O218" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P218" s="3"/>
+    </row>
+    <row r="219" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>318</v>
       </c>
@@ -11867,9 +12469,12 @@
       <c r="N219" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O219" s="3"/>
-    </row>
-    <row r="220" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+      <c r="O219" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P219" s="3"/>
+    </row>
+    <row r="220" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>318</v>
       </c>
@@ -11912,11 +12517,14 @@
       <c r="N220" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O220" s="3" t="s">
+      <c r="O220" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P220" s="3" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>318</v>
       </c>
@@ -11959,9 +12567,12 @@
       <c r="N221" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O221" s="3"/>
-    </row>
-    <row r="222" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O221" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P221" s="3"/>
+    </row>
+    <row r="222" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>318</v>
       </c>
@@ -12004,9 +12615,12 @@
       <c r="N222" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O222" s="3"/>
-    </row>
-    <row r="223" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O222" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P222" s="3"/>
+    </row>
+    <row r="223" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>318</v>
       </c>
@@ -12049,9 +12663,12 @@
       <c r="N223" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O223" s="3"/>
-    </row>
-    <row r="224" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O223" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P223" s="3"/>
+    </row>
+    <row r="224" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>318</v>
       </c>
@@ -12094,11 +12711,14 @@
       <c r="N224" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O224" s="3" t="s">
+      <c r="O224" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P224" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>318</v>
       </c>
@@ -12141,9 +12761,12 @@
       <c r="N225" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O225" s="3"/>
-    </row>
-    <row r="226" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O225" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P225" s="3"/>
+    </row>
+    <row r="226" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>318</v>
       </c>
@@ -12186,9 +12809,12 @@
       <c r="N226" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O226" s="3"/>
-    </row>
-    <row r="227" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O226" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P226" s="3"/>
+    </row>
+    <row r="227" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>318</v>
       </c>
@@ -12231,11 +12857,14 @@
       <c r="N227" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O227" s="3" t="s">
+      <c r="O227" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P227" s="3" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>318</v>
       </c>
@@ -12278,9 +12907,12 @@
       <c r="N228" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O228" s="3"/>
-    </row>
-    <row r="229" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+      <c r="O228" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P228" s="3"/>
+    </row>
+    <row r="229" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>318</v>
       </c>
@@ -12323,11 +12955,14 @@
       <c r="N229" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O229" s="3" t="s">
+      <c r="O229" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P229" s="3" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>318</v>
       </c>
@@ -12370,11 +13005,14 @@
       <c r="N230" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O230" s="3" t="s">
+      <c r="O230" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P230" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="231" spans="1:15" ht="272" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" ht="272" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>318</v>
       </c>
@@ -12417,11 +13055,14 @@
       <c r="N231" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O231" s="3" t="s">
+      <c r="O231" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P231" s="3" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>318</v>
       </c>
@@ -12464,9 +13105,12 @@
       <c r="N232" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O232" s="3"/>
-    </row>
-    <row r="233" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O232" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P232" s="3"/>
+    </row>
+    <row r="233" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>318</v>
       </c>
@@ -12509,11 +13153,14 @@
       <c r="N233" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O233" s="3" t="s">
+      <c r="O233" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P233" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>318</v>
       </c>
@@ -12556,9 +13203,12 @@
       <c r="N234" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O234" s="3"/>
-    </row>
-    <row r="235" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O234" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P234" s="3"/>
+    </row>
+    <row r="235" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>318</v>
       </c>
@@ -12601,9 +13251,12 @@
       <c r="N235" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O235" s="3"/>
-    </row>
-    <row r="236" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O235" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P235" s="3"/>
+    </row>
+    <row r="236" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>318</v>
       </c>
@@ -12646,11 +13299,14 @@
       <c r="N236" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O236" s="3" t="s">
+      <c r="O236" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P236" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>318</v>
       </c>
@@ -12675,11 +13331,12 @@
       <c r="L237" s="3"/>
       <c r="M237" s="3"/>
       <c r="N237" s="3"/>
-      <c r="O237" s="3" t="s">
+      <c r="O237" s="4"/>
+      <c r="P237" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>318</v>
       </c>
@@ -12714,11 +13371,12 @@
       </c>
       <c r="M238" s="3"/>
       <c r="N238" s="3"/>
-      <c r="O238" s="3" t="s">
+      <c r="O238" s="4"/>
+      <c r="P238" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16" ht="112" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>318</v>
       </c>
@@ -12755,11 +13413,12 @@
         <v>18</v>
       </c>
       <c r="N239" s="3"/>
-      <c r="O239" s="3" t="s">
+      <c r="O239" s="4"/>
+      <c r="P239" s="3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
         <v>318</v>
       </c>
@@ -12802,11 +13461,14 @@
       <c r="N240" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O240" s="3" t="s">
+      <c r="O240" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P240" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>318</v>
       </c>
@@ -12839,9 +13501,10 @@
       <c r="L241" s="3"/>
       <c r="M241" s="3"/>
       <c r="N241" s="3"/>
-      <c r="O241" s="3"/>
-    </row>
-    <row r="242" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+      <c r="O241" s="4"/>
+      <c r="P241" s="3"/>
+    </row>
+    <row r="242" spans="1:16" ht="96" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>318</v>
       </c>
@@ -12884,11 +13547,14 @@
       <c r="N242" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O242" s="3" t="s">
+      <c r="O242" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P242" s="3" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>318</v>
       </c>
@@ -12931,11 +13597,14 @@
       <c r="N243" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O243" s="3" t="s">
+      <c r="O243" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P243" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>411</v>
       </c>
@@ -12960,9 +13629,12 @@
       <c r="L244" s="3"/>
       <c r="M244" s="3"/>
       <c r="N244" s="3"/>
-      <c r="O244" s="3"/>
-    </row>
-    <row r="245" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O244" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P244" s="3"/>
+    </row>
+    <row r="245" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>411</v>
       </c>
@@ -12993,11 +13665,14 @@
         <v>18</v>
       </c>
       <c r="N245" s="3"/>
-      <c r="O245" s="3" t="s">
+      <c r="O245" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P245" s="3" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>411</v>
       </c>
@@ -13022,9 +13697,12 @@
       <c r="L246" s="3"/>
       <c r="M246" s="3"/>
       <c r="N246" s="3"/>
-      <c r="O246" s="3"/>
-    </row>
-    <row r="247" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O246" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P246" s="3"/>
+    </row>
+    <row r="247" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>411</v>
       </c>
@@ -13049,9 +13727,12 @@
       <c r="L247" s="3"/>
       <c r="M247" s="3"/>
       <c r="N247" s="3"/>
-      <c r="O247" s="3"/>
-    </row>
-    <row r="248" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O247" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P247" s="3"/>
+    </row>
+    <row r="248" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>411</v>
       </c>
@@ -13076,9 +13757,12 @@
       <c r="L248" s="3"/>
       <c r="M248" s="3"/>
       <c r="N248" s="3"/>
-      <c r="O248" s="3"/>
-    </row>
-    <row r="249" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O248" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P248" s="3"/>
+    </row>
+    <row r="249" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>411</v>
       </c>
@@ -13103,9 +13787,12 @@
       <c r="L249" s="3"/>
       <c r="M249" s="3"/>
       <c r="N249" s="3"/>
-      <c r="O249" s="3"/>
-    </row>
-    <row r="250" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O249" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P249" s="3"/>
+    </row>
+    <row r="250" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>411</v>
       </c>
@@ -13130,9 +13817,12 @@
       <c r="L250" s="3"/>
       <c r="M250" s="3"/>
       <c r="N250" s="3"/>
-      <c r="O250" s="3"/>
-    </row>
-    <row r="251" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O250" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P250" s="3"/>
+    </row>
+    <row r="251" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>411</v>
       </c>
@@ -13157,9 +13847,12 @@
       <c r="L251" s="3"/>
       <c r="M251" s="3"/>
       <c r="N251" s="3"/>
-      <c r="O251" s="3"/>
-    </row>
-    <row r="252" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O251" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P251" s="3"/>
+    </row>
+    <row r="252" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>411</v>
       </c>
@@ -13184,9 +13877,12 @@
       <c r="L252" s="3"/>
       <c r="M252" s="3"/>
       <c r="N252" s="3"/>
-      <c r="O252" s="3"/>
-    </row>
-    <row r="253" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O252" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P252" s="3"/>
+    </row>
+    <row r="253" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>411</v>
       </c>
@@ -13211,9 +13907,12 @@
       <c r="L253" s="3"/>
       <c r="M253" s="3"/>
       <c r="N253" s="3"/>
-      <c r="O253" s="3"/>
-    </row>
-    <row r="254" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O253" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P253" s="3"/>
+    </row>
+    <row r="254" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>411</v>
       </c>
@@ -13238,9 +13937,12 @@
       <c r="L254" s="3"/>
       <c r="M254" s="3"/>
       <c r="N254" s="3"/>
-      <c r="O254" s="3"/>
-    </row>
-    <row r="255" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O254" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P254" s="3"/>
+    </row>
+    <row r="255" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>411</v>
       </c>
@@ -13265,9 +13967,12 @@
       <c r="L255" s="3"/>
       <c r="M255" s="3"/>
       <c r="N255" s="3"/>
-      <c r="O255" s="3"/>
-    </row>
-    <row r="256" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="O255" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P255" s="3"/>
+    </row>
+    <row r="256" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>411</v>
       </c>
@@ -13310,11 +14015,14 @@
       <c r="N256" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O256" s="3" t="s">
+      <c r="O256" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P256" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>427</v>
       </c>
@@ -13355,11 +14063,14 @@
       <c r="N257" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O257" s="3" t="s">
+      <c r="O257" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P257" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>427</v>
       </c>
@@ -13382,11 +14093,14 @@
       <c r="L258" s="3"/>
       <c r="M258" s="3"/>
       <c r="N258" s="3"/>
-      <c r="O258" s="3" t="s">
+      <c r="O258" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P258" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>427</v>
       </c>
@@ -13411,11 +14125,14 @@
       <c r="L259" s="3"/>
       <c r="M259" s="3"/>
       <c r="N259" s="3"/>
-      <c r="O259" s="3" t="s">
+      <c r="O259" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P259" s="3" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>427</v>
       </c>
@@ -13440,9 +14157,10 @@
       <c r="L260" s="3"/>
       <c r="M260" s="3"/>
       <c r="N260" s="3"/>
-      <c r="O260" s="3"/>
-    </row>
-    <row r="261" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O260" s="4"/>
+      <c r="P260" s="3"/>
+    </row>
+    <row r="261" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>427</v>
       </c>
@@ -13467,11 +14185,14 @@
       <c r="L261" s="3"/>
       <c r="M261" s="3"/>
       <c r="N261" s="3"/>
-      <c r="O261" s="3" t="s">
+      <c r="O261" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P261" s="3" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>427</v>
       </c>
@@ -13502,11 +14223,14 @@
         <v>18</v>
       </c>
       <c r="N262" s="3"/>
-      <c r="O262" s="3" t="s">
+      <c r="O262" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P262" s="3" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>427</v>
       </c>
@@ -13533,9 +14257,12 @@
       <c r="L263" s="3"/>
       <c r="M263" s="3"/>
       <c r="N263" s="3"/>
-      <c r="O263" s="3"/>
-    </row>
-    <row r="264" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+      <c r="O263" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P263" s="3"/>
+    </row>
+    <row r="264" spans="1:16" ht="96" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>427</v>
       </c>
@@ -13558,11 +14285,14 @@
       <c r="L264" s="3"/>
       <c r="M264" s="3"/>
       <c r="N264" s="3"/>
-      <c r="O264" s="3" t="s">
+      <c r="O264" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P264" s="3" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="176" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:16" ht="176" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>427</v>
       </c>
@@ -13603,11 +14333,14 @@
       <c r="N265" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O265" s="3" t="s">
+      <c r="O265" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P265" s="3" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>427</v>
       </c>
@@ -13634,11 +14367,12 @@
       <c r="L266" s="3"/>
       <c r="M266" s="3"/>
       <c r="N266" s="3"/>
-      <c r="O266" s="3" t="s">
+      <c r="O266" s="4"/>
+      <c r="P266" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>427</v>
       </c>
@@ -13675,11 +14409,12 @@
         <v>18</v>
       </c>
       <c r="N267" s="3"/>
-      <c r="O267" s="3" t="s">
+      <c r="O267" s="4"/>
+      <c r="P267" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="365" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16" ht="365" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>427</v>
       </c>
@@ -13706,11 +14441,12 @@
       <c r="L268" s="3"/>
       <c r="M268" s="3"/>
       <c r="N268" s="3"/>
-      <c r="O268" s="3" t="s">
+      <c r="O268" s="4"/>
+      <c r="P268" s="3" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>427</v>
       </c>
@@ -13735,11 +14471,12 @@
       <c r="L269" s="3"/>
       <c r="M269" s="3"/>
       <c r="N269" s="3"/>
-      <c r="O269" s="3" t="s">
+      <c r="O269" s="4"/>
+      <c r="P269" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>427</v>
       </c>
@@ -13764,11 +14501,12 @@
       <c r="L270" s="3"/>
       <c r="M270" s="3"/>
       <c r="N270" s="3"/>
-      <c r="O270" s="3" t="s">
+      <c r="O270" s="4"/>
+      <c r="P270" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>427</v>
       </c>
@@ -13795,11 +14533,12 @@
       <c r="L271" s="3"/>
       <c r="M271" s="3"/>
       <c r="N271" s="3"/>
-      <c r="O271" s="3" t="s">
+      <c r="O271" s="4"/>
+      <c r="P271" s="3" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>427</v>
       </c>
@@ -13822,9 +14561,12 @@
       <c r="L272" s="3"/>
       <c r="M272" s="3"/>
       <c r="N272" s="3"/>
-      <c r="O272" s="3"/>
-    </row>
-    <row r="273" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="O272" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P272" s="3"/>
+    </row>
+    <row r="273" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>427</v>
       </c>
@@ -13849,11 +14591,12 @@
       <c r="L273" s="3"/>
       <c r="M273" s="3"/>
       <c r="N273" s="3"/>
-      <c r="O273" s="3" t="s">
+      <c r="O273" s="4"/>
+      <c r="P273" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>427</v>
       </c>
@@ -13896,11 +14639,14 @@
       <c r="N274" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O274" s="3" t="s">
+      <c r="O274" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P274" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>427</v>
       </c>
@@ -13927,11 +14673,12 @@
       <c r="L275" s="3"/>
       <c r="M275" s="3"/>
       <c r="N275" s="3"/>
-      <c r="O275" s="3" t="s">
+      <c r="O275" s="4"/>
+      <c r="P275" s="3" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>427</v>
       </c>
@@ -13974,11 +14721,14 @@
       <c r="N276" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O276" s="3" t="s">
+      <c r="O276" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P276" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>427</v>
       </c>
@@ -14005,11 +14755,12 @@
       <c r="L277" s="3"/>
       <c r="M277" s="3"/>
       <c r="N277" s="3"/>
-      <c r="O277" s="3" t="s">
+      <c r="O277" s="4"/>
+      <c r="P277" s="3" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
         <v>427</v>
       </c>
@@ -14034,11 +14785,12 @@
       <c r="L278" s="3"/>
       <c r="M278" s="3"/>
       <c r="N278" s="3"/>
-      <c r="O278" s="3" t="s">
+      <c r="O278" s="4"/>
+      <c r="P278" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>427</v>
       </c>
@@ -14065,11 +14817,12 @@
       <c r="L279" s="3"/>
       <c r="M279" s="3"/>
       <c r="N279" s="3"/>
-      <c r="O279" s="3" t="s">
+      <c r="O279" s="4"/>
+      <c r="P279" s="3" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="280" spans="1:15" ht="144" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16" ht="144" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>427</v>
       </c>
@@ -14094,7 +14847,8 @@
       <c r="L280" s="3"/>
       <c r="M280" s="3"/>
       <c r="N280" s="3"/>
-      <c r="O280" s="3" t="s">
+      <c r="O280" s="4"/>
+      <c r="P280" s="3" t="s">
         <v>464</v>
       </c>
     </row>

</xml_diff>